<commit_message>
feat: Enhance freight calculation with score-based matrix and additional configurations
- Added a new 'score' field to the CanalVenda model for improved freight calculations based on score metrics.
- Updated the obter_frete method to include dimensions and score in freight calculations.
- Introduced a new freight table type 'matriz_score' to support calculations based on weight and score.
- Enhanced the TabelaFrete model to include options for handling freight rules exceeding 1 meter.
- Updated templates and forms to accommodate new fields and options for freight rules, including score and exceeding dimensions.
- Implemented migration scripts to add new fields and update existing models accordingly.
</commit_message>
<xml_diff>
--- a/Tabela Frete/Shein.xlsx
+++ b/Tabela Frete/Shein.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows\3D Objects\Precos\Tabela Frete\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC8A1AC-7A5A-4FCB-BF69-313A12ACC8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D996114-23B2-43A1-A302-D8D015E447E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,15 +20,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>inicio (kg)</t>
-  </si>
-  <si>
-    <t>fim (kg)</t>
-  </si>
-  <si>
-    <t>valor_frete (R$)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>peso_inicio</t>
+  </si>
+  <si>
+    <t>peso_fim</t>
+  </si>
+  <si>
+    <t>preco_inicio</t>
+  </si>
+  <si>
+    <t>preco_fim</t>
+  </si>
+  <si>
+    <t>score_inicio</t>
+  </si>
+  <si>
+    <t>score_fim</t>
+  </si>
+  <si>
+    <t>valor_frete</t>
+  </si>
+  <si>
+    <t>ordem</t>
+  </si>
+  <si>
+    <t>excedente (0 ou 1)</t>
   </si>
 </sst>
 </file>
@@ -67,9 +85,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -373,15 +390,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C13"/>
+      <selection activeCell="I2" sqref="I2:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -391,137 +419,191 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
         <v>0.3</v>
       </c>
-      <c r="C2" s="1">
+      <c r="G2">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>0.3</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>0.6</v>
       </c>
-      <c r="C3" s="1">
+      <c r="G3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>0.6</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>0.9</v>
       </c>
-      <c r="C4" s="1">
+      <c r="G4">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>0.9</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>1.2</v>
       </c>
-      <c r="C5" s="1">
+      <c r="G5">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>1.2</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>1.5</v>
       </c>
-      <c r="C6" s="1">
+      <c r="G6">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>1.5</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>2</v>
       </c>
-      <c r="C7" s="1">
+      <c r="G7">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>2</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>5</v>
       </c>
-      <c r="C8" s="1">
+      <c r="G8">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>5</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>9</v>
       </c>
-      <c r="C9" s="1">
+      <c r="G9">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>13</v>
       </c>
-      <c r="C10" s="1">
+      <c r="G10">
         <v>63</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>13</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>17</v>
       </c>
-      <c r="C11" s="1">
+      <c r="G11">
         <v>73</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>17</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>23</v>
       </c>
-      <c r="C12" s="1">
+      <c r="G12">
         <v>89</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="I12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>23</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>30</v>
       </c>
-      <c r="C13" s="1">
+      <c r="G13">
         <v>106</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>